<commit_message>
<Upd><UploadFTAMaster><Update Insert Function Upload>
</commit_message>
<xml_diff>
--- a/PECGI_SPC/Template/Template FTA Master.xlsx
+++ b/PECGI_SPC/Template/Template FTA Master.xlsx
@@ -29,7 +29,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>* Type must be filled</t>
+          <t>* Type must be filled
+Ex : BR2450A
+For format Type can be view on Menu A020 - Item Check By Type</t>
         </r>
       </text>
     </comment>
@@ -43,7 +45,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>* Item Check Must Be Filled</t>
+          <t>* Item Check Must Be Filled
+Ex : IC020
+For format Item Check can be view on Menu A020 - Item Check By Type</t>
         </r>
       </text>
     </comment>
@@ -57,7 +61,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>* FTA ID Must Be Filled</t>
+          <t>* FTA ID Must Be Filled
+Ex : IC020-1</t>
         </r>
       </text>
     </comment>
@@ -565,7 +570,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>